<commit_message>
add scripts: index calculation
</commit_message>
<xml_diff>
--- a/data/myobject.xlsx
+++ b/data/myobject.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="12030"/>
+    <workbookView windowWidth="13440" windowHeight="12030"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="112">
   <si>
     <r>
       <rPr>
@@ -342,39 +342,6 @@
         <rFont val="Arial"/>
         <charset val="134"/>
       </rPr>
-      <t>(120, 120, 70)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>#787846</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>earth;ground</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
       <t>(204, 255, 4)</t>
     </r>
   </si>
@@ -464,39 +431,6 @@
         <charset val="134"/>
       </rPr>
       <t>car;auto;automobile;machine;motorcar</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>(255, 9, 224)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>#FF09E0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>house</t>
     </r>
   </si>
   <si>
@@ -1313,7 +1247,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1333,13 +1267,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -1486,7 +1413,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="70">
+  <fills count="68">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1543,12 +1470,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF787846"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFCCFF04"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1562,12 +1483,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0066C8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF09E0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2026,85 +1941,91 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="39" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="40" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="41" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="41" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="42" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="39" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="40" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2113,10 +2034,10 @@
     <xf numFmtId="0" fontId="21" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="52" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="52" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="53" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2125,10 +2046,10 @@
     <xf numFmtId="0" fontId="21" fillId="54" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="55" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="56" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="55" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="56" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="57" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2137,10 +2058,10 @@
     <xf numFmtId="0" fontId="21" fillId="58" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="59" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="60" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="59" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="60" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="61" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2149,10 +2070,10 @@
     <xf numFmtId="0" fontId="21" fillId="62" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="63" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="64" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="63" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="64" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="65" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2161,17 +2082,11 @@
     <xf numFmtId="0" fontId="21" fillId="66" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="67" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="68" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="69" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="67" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2268,13 +2183,13 @@
     <xf numFmtId="0" fontId="2" fillId="30" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="31" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
@@ -2285,12 +2200,6 @@
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="37" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="38" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -2612,10 +2521,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="5"/>
@@ -2661,7 +2570,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" ht="25.75" spans="1:5">
+    <row r="3" ht="15.25" spans="1:5">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2736,7 +2645,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" ht="25.75" spans="1:5">
+    <row r="8" ht="15.25" spans="1:5">
       <c r="A8" s="4">
         <v>12</v>
       </c>
@@ -2766,9 +2675,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" ht="15.25" spans="1:5">
+    <row r="10" spans="1:5">
       <c r="A10" s="4">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>30</v>
@@ -2781,9 +2690,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" ht="15.25" spans="1:5">
+    <row r="11" spans="1:5">
       <c r="A11" s="4">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>33</v>
@@ -2796,9 +2705,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" ht="15.25" spans="1:5">
+    <row r="12" spans="1:5">
       <c r="A12" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>36</v>
@@ -2811,9 +2720,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" ht="15.25" spans="1:5">
+    <row r="13" spans="1:5">
       <c r="A13" s="4">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>39</v>
@@ -2826,9 +2735,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" ht="15.25" spans="1:5">
+    <row r="14" spans="1:5">
       <c r="A14" s="4">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>42</v>
@@ -2843,7 +2752,7 @@
     </row>
     <row r="15" ht="15.25" spans="1:5">
       <c r="A15" s="4">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>45</v>
@@ -2858,7 +2767,7 @@
     </row>
     <row r="16" ht="15.25" spans="1:5">
       <c r="A16" s="4">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>48</v>
@@ -2873,7 +2782,7 @@
     </row>
     <row r="17" ht="15.25" spans="1:5">
       <c r="A17" s="4">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>51</v>
@@ -2888,7 +2797,7 @@
     </row>
     <row r="18" ht="15.25" spans="1:5">
       <c r="A18" s="4">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>54</v>
@@ -2903,7 +2812,7 @@
     </row>
     <row r="19" ht="15.25" spans="1:5">
       <c r="A19" s="4">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>57</v>
@@ -2918,52 +2827,52 @@
     </row>
     <row r="20" ht="15.25" spans="1:5">
       <c r="A20" s="4">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" s="23"/>
-      <c r="E20" s="6" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="21" ht="15.25" spans="1:5">
       <c r="A21" s="4">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="23"/>
+      <c r="E21" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" s="24"/>
-      <c r="E21" s="6" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="22" ht="15.25" spans="1:5">
       <c r="A22" s="4">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="9"/>
+        <v>65</v>
+      </c>
+      <c r="D22" s="24"/>
       <c r="E22" s="6" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="23" ht="15.25" spans="1:5">
       <c r="A23" s="4">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>67</v>
@@ -2978,7 +2887,7 @@
     </row>
     <row r="24" ht="15.25" spans="1:5">
       <c r="A24" s="4">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>70</v>
@@ -2991,9 +2900,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" ht="15.25" spans="1:5">
+    <row r="25" ht="25.75" spans="1:5">
       <c r="A25" s="4">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>73</v>
@@ -3008,7 +2917,7 @@
     </row>
     <row r="26" ht="15.25" spans="1:5">
       <c r="A26" s="4">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>76</v>
@@ -3021,9 +2930,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" ht="25.75" spans="1:5">
+    <row r="27" ht="15.25" spans="1:5">
       <c r="A27" s="4">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>79</v>
@@ -3038,7 +2947,7 @@
     </row>
     <row r="28" ht="15.25" spans="1:5">
       <c r="A28" s="4">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>82</v>
@@ -3053,7 +2962,7 @@
     </row>
     <row r="29" ht="15.25" spans="1:5">
       <c r="A29" s="4">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>85</v>
@@ -3068,7 +2977,7 @@
     </row>
     <row r="30" ht="15.25" spans="1:5">
       <c r="A30" s="4">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>88</v>
@@ -3083,7 +2992,7 @@
     </row>
     <row r="31" ht="15.25" spans="1:5">
       <c r="A31" s="4">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>91</v>
@@ -3092,13 +3001,13 @@
         <v>92</v>
       </c>
       <c r="D31" s="33"/>
-      <c r="E31" s="6" t="s">
+      <c r="E31" s="34" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="32" ht="15.25" spans="1:5">
       <c r="A32" s="4">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>94</v>
@@ -3106,14 +3015,14 @@
       <c r="C32" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D32" s="34"/>
+      <c r="D32" s="35"/>
       <c r="E32" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="33" ht="15.25" spans="1:5">
       <c r="A33" s="4">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>97</v>
@@ -3121,14 +3030,14 @@
       <c r="C33" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D33" s="35"/>
-      <c r="E33" s="36" t="s">
+      <c r="D33" s="36"/>
+      <c r="E33" s="6" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="34" ht="15.25" spans="1:5">
       <c r="A34" s="4">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>100</v>
@@ -3141,9 +3050,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="35" ht="15.25" spans="1:5">
+    <row r="35" ht="25.75" spans="1:5">
       <c r="A35" s="4">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>103</v>
@@ -3156,9 +3065,9 @@
         <v>105</v>
       </c>
     </row>
-    <row r="36" ht="15.25" spans="1:5">
+    <row r="36" ht="25.75" spans="1:5">
       <c r="A36" s="4">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>106</v>
@@ -3171,9 +3080,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="37" ht="25.75" spans="1:5">
+    <row r="37" ht="15.25" spans="1:5">
       <c r="A37" s="4">
-        <v>96</v>
+        <v>137</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>109</v>
@@ -3184,36 +3093,6 @@
       <c r="D37" s="40"/>
       <c r="E37" s="6" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="38" ht="25.75" spans="1:5">
-      <c r="A38" s="4">
-        <v>97</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D38" s="41"/>
-      <c r="E38" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="39" ht="15.25" spans="1:5">
-      <c r="A39" s="4">
-        <v>137</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D39" s="42"/>
-      <c r="E39" s="6" t="s">
-        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>